<commit_message>
improved cholera verification, assessment and follow up form
</commit_message>
<xml_diff>
--- a/forms/app/cholera_verification.xlsx
+++ b/forms/app/cholera_verification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -264,7 +264,51 @@
     <t xml:space="preserve">confirm_case</t>
   </si>
   <si>
-    <t xml:space="preserve">Is this a confirmed cholera case?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">patient_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">} C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">holera case confirmed?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -276,7 +320,7 @@
     <t xml:space="preserve">reason</t>
   </si>
   <si>
-    <t xml:space="preserve">Requested for Immediate Confirmation of Suspected Cholera Case.</t>
+    <t xml:space="preserve">&lt;p style=”color:red”&gt;Requested for Immediate Confirmation of Suspected Cholera Case.&lt;/p&gt;</t>
   </si>
   <si>
     <r>
@@ -405,7 +449,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -440,6 +484,18 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -652,7 +708,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,7 +716,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,55 +736,55 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,7 +792,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,11 +800,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -831,13 +887,13 @@
   </sheetPr>
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="W32" activeCellId="1" sqref="A4:C11 W32"/>
+      <selection pane="bottomLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.42"/>
@@ -3419,11 +3475,11 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="36.39"/>
@@ -3770,10 +3826,10 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:C11"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.01"/>
@@ -3831,7 +3887,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>45259.7242698255</v>
+        <v>45261.3316881744</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>102</v>

</xml_diff>